<commit_message>
add flu model select
</commit_message>
<xml_diff>
--- a/outcome/model_select_flu.xlsx
+++ b/outcome/model_select_flu.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kanggle-my.sharepoint.com/personal/phonedata_kanggle_onmicrosoft_com/Documents/XMU/likangguo/2022/OK 11 COVID_impact_luoli/code/outcome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kanggle-my.sharepoint.com/personal/phonedata_kanggle_onmicrosoft_com/Documents/XMU/likangguo/2022/11 COVID_impact_luoli/code/outcome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_ABAA72291DE16DA756A53C4E5F7A0EC4EAD94F12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64499F66-6B00-4189-9B74-EDF66BA536F1}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_ABAA72291DE16DA756A53C4E5F7A0EC4EAD94F12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B435F2C-333D-487A-876C-7748C138E154}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3948" yWindow="2892" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="result" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="39">
   <si>
     <t>Method</t>
   </si>
@@ -120,12 +121,35 @@
   <si>
     <t>Typhus</t>
   </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>Final</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,16 +164,48 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,12 +213,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -178,6 +250,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -461,17 +537,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C371" sqref="C371"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -493,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -504,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -515,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -526,7 +602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -537,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -548,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -559,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -570,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -581,7 +657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -592,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -603,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -614,7 +690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -625,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -636,7 +712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -647,7 +723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -658,7 +734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -669,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -680,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -691,7 +767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -702,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -713,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -724,7 +800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -735,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -746,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -757,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -768,7 +844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -779,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -790,7 +866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -801,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -812,7 +888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -823,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -834,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -845,7 +921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -856,7 +932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -867,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -878,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -889,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -900,7 +976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -911,7 +987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -922,7 +998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -933,7 +1009,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -944,7 +1020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -955,7 +1031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -966,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -977,7 +1053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -988,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -1021,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -1043,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1065,7 +1141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1131,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1229,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1164,7 +1240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1175,7 +1251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1262,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1273,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -1230,7 +1306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1339,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -1274,7 +1350,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1285,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1329,7 +1405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -1362,7 +1438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -1373,7 +1449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -1384,7 +1460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -1406,7 +1482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>9</v>
       </c>
@@ -1439,7 +1515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1526,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -1472,7 +1548,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -1494,7 +1570,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +1592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -1549,7 +1625,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -1560,7 +1636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +1647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -1582,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -1593,7 +1669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -1604,7 +1680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -1626,7 +1702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -1637,7 +1713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -1681,7 +1757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -1692,7 +1768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -1747,7 +1823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>7</v>
       </c>
@@ -1758,7 +1834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -1769,7 +1845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -1780,7 +1856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -1791,7 +1867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -1802,7 +1878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -1813,7 +1889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -1824,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -1835,7 +1911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -1857,7 +1933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -1879,7 +1955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +1977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +1988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -1923,7 +1999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -1934,7 +2010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>7</v>
       </c>
@@ -1945,7 +2021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -1956,7 +2032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>7</v>
       </c>
@@ -1967,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +2054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -1989,7 +2065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -2000,7 +2076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -2011,7 +2087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -2022,7 +2098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -2033,7 +2109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -2055,7 +2131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -2066,7 +2142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -2088,7 +2164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -2099,7 +2175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -2121,7 +2197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>7</v>
       </c>
@@ -2143,7 +2219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2230,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>7</v>
       </c>
@@ -2165,7 +2241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>8</v>
       </c>
@@ -2176,7 +2252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -2187,7 +2263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -2198,7 +2274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -2220,7 +2296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>9</v>
       </c>
@@ -2231,7 +2307,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>3</v>
       </c>
@@ -2242,7 +2318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>3</v>
       </c>
@@ -2253,7 +2329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>5</v>
       </c>
@@ -2275,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>5</v>
       </c>
@@ -2286,7 +2362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>5</v>
       </c>
@@ -2297,7 +2373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>6</v>
       </c>
@@ -2308,7 +2384,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>6</v>
       </c>
@@ -2319,7 +2395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>6</v>
       </c>
@@ -2330,7 +2406,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>7</v>
       </c>
@@ -2341,7 +2417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>7</v>
       </c>
@@ -2352,7 +2428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>7</v>
       </c>
@@ -2363,7 +2439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -2374,7 +2450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -2385,7 +2461,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -2396,7 +2472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>9</v>
       </c>
@@ -2407,7 +2483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -2418,7 +2494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>9</v>
       </c>
@@ -2429,7 +2505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>3</v>
       </c>
@@ -2440,7 +2516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>3</v>
       </c>
@@ -2451,7 +2527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>3</v>
       </c>
@@ -2462,7 +2538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -2473,7 +2549,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>5</v>
       </c>
@@ -2484,7 +2560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>5</v>
       </c>
@@ -2495,7 +2571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>6</v>
       </c>
@@ -2506,7 +2582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>6</v>
       </c>
@@ -2517,7 +2593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>6</v>
       </c>
@@ -2528,7 +2604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>7</v>
       </c>
@@ -2550,7 +2626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>7</v>
       </c>
@@ -2561,7 +2637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>8</v>
       </c>
@@ -2572,7 +2648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>8</v>
       </c>
@@ -2583,7 +2659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>8</v>
       </c>
@@ -2594,7 +2670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>9</v>
       </c>
@@ -2605,7 +2681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -2616,7 +2692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>3</v>
       </c>
@@ -2638,7 +2714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>3</v>
       </c>
@@ -2649,7 +2725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>3</v>
       </c>
@@ -2660,7 +2736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>5</v>
       </c>
@@ -2671,7 +2747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>5</v>
       </c>
@@ -2682,7 +2758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>5</v>
       </c>
@@ -2693,7 +2769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>6</v>
       </c>
@@ -2704,7 +2780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>6</v>
       </c>
@@ -2715,7 +2791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>6</v>
       </c>
@@ -2726,7 +2802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>7</v>
       </c>
@@ -2737,7 +2813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>7</v>
       </c>
@@ -2748,7 +2824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>7</v>
       </c>
@@ -2759,7 +2835,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>8</v>
       </c>
@@ -2770,7 +2846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>8</v>
       </c>
@@ -2781,7 +2857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>8</v>
       </c>
@@ -2792,7 +2868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>9</v>
       </c>
@@ -2803,7 +2879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -2814,7 +2890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>9</v>
       </c>
@@ -2825,7 +2901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>3</v>
       </c>
@@ -2836,7 +2912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>3</v>
       </c>
@@ -2847,7 +2923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>3</v>
       </c>
@@ -2858,7 +2934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>5</v>
       </c>
@@ -2869,7 +2945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>5</v>
       </c>
@@ -2880,7 +2956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>5</v>
       </c>
@@ -2891,7 +2967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>6</v>
       </c>
@@ -2902,7 +2978,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>6</v>
       </c>
@@ -2913,7 +2989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>6</v>
       </c>
@@ -2924,7 +3000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>7</v>
       </c>
@@ -2935,7 +3011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>7</v>
       </c>
@@ -2946,7 +3022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>7</v>
       </c>
@@ -2957,7 +3033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>8</v>
       </c>
@@ -2968,7 +3044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>8</v>
       </c>
@@ -2979,7 +3055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>8</v>
       </c>
@@ -2990,7 +3066,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -3001,7 +3077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -3012,7 +3088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -3023,7 +3099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>3</v>
       </c>
@@ -3034,7 +3110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +3121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>3</v>
       </c>
@@ -3056,7 +3132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>5</v>
       </c>
@@ -3067,7 +3143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>5</v>
       </c>
@@ -3078,7 +3154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>5</v>
       </c>
@@ -3089,7 +3165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>6</v>
       </c>
@@ -3100,7 +3176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>6</v>
       </c>
@@ -3111,7 +3187,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>6</v>
       </c>
@@ -3122,7 +3198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>7</v>
       </c>
@@ -3133,7 +3209,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>7</v>
       </c>
@@ -3144,7 +3220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>7</v>
       </c>
@@ -3155,7 +3231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>8</v>
       </c>
@@ -3166,7 +3242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>8</v>
       </c>
@@ -3177,7 +3253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>8</v>
       </c>
@@ -3188,7 +3264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -3199,7 +3275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -3210,7 +3286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>9</v>
       </c>
@@ -3221,7 +3297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>3</v>
       </c>
@@ -3232,7 +3308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>3</v>
       </c>
@@ -3243,7 +3319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>3</v>
       </c>
@@ -3254,7 +3330,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>5</v>
       </c>
@@ -3265,7 +3341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>5</v>
       </c>
@@ -3276,7 +3352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>5</v>
       </c>
@@ -3287,7 +3363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>6</v>
       </c>
@@ -3298,7 +3374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>6</v>
       </c>
@@ -3309,7 +3385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>6</v>
       </c>
@@ -3320,7 +3396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>7</v>
       </c>
@@ -3331,7 +3407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>7</v>
       </c>
@@ -3342,7 +3418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>7</v>
       </c>
@@ -3353,7 +3429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>8</v>
       </c>
@@ -3364,7 +3440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>8</v>
       </c>
@@ -3375,7 +3451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>8</v>
       </c>
@@ -3386,7 +3462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>9</v>
       </c>
@@ -3397,7 +3473,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>9</v>
       </c>
@@ -3408,7 +3484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>9</v>
       </c>
@@ -3419,7 +3495,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>3</v>
       </c>
@@ -3430,7 +3506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>3</v>
       </c>
@@ -3441,7 +3517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>3</v>
       </c>
@@ -3452,7 +3528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>5</v>
       </c>
@@ -3463,7 +3539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>5</v>
       </c>
@@ -3474,7 +3550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>5</v>
       </c>
@@ -3485,7 +3561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>6</v>
       </c>
@@ -3496,7 +3572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>6</v>
       </c>
@@ -3507,7 +3583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>6</v>
       </c>
@@ -3518,7 +3594,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>7</v>
       </c>
@@ -3529,7 +3605,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>7</v>
       </c>
@@ -3540,7 +3616,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>7</v>
       </c>
@@ -3551,7 +3627,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>8</v>
       </c>
@@ -3562,7 +3638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>8</v>
       </c>
@@ -3573,7 +3649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>8</v>
       </c>
@@ -3584,7 +3660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>9</v>
       </c>
@@ -3595,7 +3671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>9</v>
       </c>
@@ -3606,7 +3682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>9</v>
       </c>
@@ -3617,7 +3693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>3</v>
       </c>
@@ -3628,7 +3704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>3</v>
       </c>
@@ -3639,7 +3715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>3</v>
       </c>
@@ -3650,7 +3726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>5</v>
       </c>
@@ -3661,7 +3737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>5</v>
       </c>
@@ -3672,7 +3748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>5</v>
       </c>
@@ -3683,7 +3759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -3694,7 +3770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>6</v>
       </c>
@@ -3705,7 +3781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>6</v>
       </c>
@@ -3716,7 +3792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>7</v>
       </c>
@@ -3727,7 +3803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>7</v>
       </c>
@@ -3738,7 +3814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>7</v>
       </c>
@@ -3749,7 +3825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>8</v>
       </c>
@@ -3760,7 +3836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>8</v>
       </c>
@@ -3771,7 +3847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>8</v>
       </c>
@@ -3782,7 +3858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>9</v>
       </c>
@@ -3793,7 +3869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>9</v>
       </c>
@@ -3804,7 +3880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>9</v>
       </c>
@@ -3815,7 +3891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>3</v>
       </c>
@@ -3826,7 +3902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>3</v>
       </c>
@@ -3837,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>3</v>
       </c>
@@ -3848,7 +3924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>5</v>
       </c>
@@ -3859,7 +3935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>5</v>
       </c>
@@ -3870,7 +3946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>5</v>
       </c>
@@ -3881,7 +3957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>6</v>
       </c>
@@ -3892,7 +3968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>6</v>
       </c>
@@ -3903,7 +3979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>6</v>
       </c>
@@ -3914,7 +3990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>7</v>
       </c>
@@ -3925,7 +4001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>7</v>
       </c>
@@ -3936,7 +4012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +4023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>8</v>
       </c>
@@ -3958,7 +4034,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>8</v>
       </c>
@@ -3969,7 +4045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>8</v>
       </c>
@@ -3980,7 +4056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>9</v>
       </c>
@@ -3991,7 +4067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>9</v>
       </c>
@@ -4002,7 +4078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>9</v>
       </c>
@@ -4013,7 +4089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>3</v>
       </c>
@@ -4024,7 +4100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>3</v>
       </c>
@@ -4035,7 +4111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>3</v>
       </c>
@@ -4046,7 +4122,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>5</v>
       </c>
@@ -4057,7 +4133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>5</v>
       </c>
@@ -4068,7 +4144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>5</v>
       </c>
@@ -4079,7 +4155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>6</v>
       </c>
@@ -4090,7 +4166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>6</v>
       </c>
@@ -4101,7 +4177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>6</v>
       </c>
@@ -4112,7 +4188,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>7</v>
       </c>
@@ -4123,7 +4199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>7</v>
       </c>
@@ -4134,7 +4210,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>7</v>
       </c>
@@ -4145,7 +4221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>8</v>
       </c>
@@ -4156,7 +4232,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>8</v>
       </c>
@@ -4167,7 +4243,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>8</v>
       </c>
@@ -4178,7 +4254,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>9</v>
       </c>
@@ -4189,7 +4265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>9</v>
       </c>
@@ -4200,7 +4276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>9</v>
       </c>
@@ -4211,7 +4287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>3</v>
       </c>
@@ -4222,7 +4298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>3</v>
       </c>
@@ -4230,7 +4306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>3</v>
       </c>
@@ -4241,7 +4317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>5</v>
       </c>
@@ -4252,7 +4328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>5</v>
       </c>
@@ -4263,7 +4339,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>5</v>
       </c>
@@ -4274,7 +4350,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>6</v>
       </c>
@@ -4285,7 +4361,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>6</v>
       </c>
@@ -4307,7 +4383,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>8</v>
       </c>
@@ -4318,7 +4394,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>8</v>
       </c>
@@ -4329,7 +4405,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>8</v>
       </c>
@@ -4340,7 +4416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>9</v>
       </c>
@@ -4351,7 +4427,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>9</v>
       </c>
@@ -4362,7 +4438,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>9</v>
       </c>
@@ -4373,7 +4449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>3</v>
       </c>
@@ -4384,7 +4460,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>3</v>
       </c>
@@ -4395,7 +4471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>3</v>
       </c>
@@ -4406,7 +4482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>5</v>
       </c>
@@ -4417,7 +4493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>5</v>
       </c>
@@ -4428,7 +4504,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>5</v>
       </c>
@@ -4439,7 +4515,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>6</v>
       </c>
@@ -4450,7 +4526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>6</v>
       </c>
@@ -4461,7 +4537,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>6</v>
       </c>
@@ -4472,7 +4548,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>7</v>
       </c>
@@ -4483,7 +4559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>7</v>
       </c>
@@ -4494,7 +4570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>7</v>
       </c>
@@ -4505,7 +4581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>8</v>
       </c>
@@ -4516,7 +4592,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>8</v>
       </c>
@@ -4527,7 +4603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>8</v>
       </c>
@@ -4538,7 +4614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>9</v>
       </c>
@@ -4549,7 +4625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>9</v>
       </c>
@@ -4560,7 +4636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>9</v>
       </c>
@@ -4571,7 +4647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>3</v>
       </c>
@@ -4582,7 +4658,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>3</v>
       </c>
@@ -4593,7 +4669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>3</v>
       </c>
@@ -4604,7 +4680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>5</v>
       </c>
@@ -4615,7 +4691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>5</v>
       </c>
@@ -4626,7 +4702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>5</v>
       </c>
@@ -4637,7 +4713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>6</v>
       </c>
@@ -4648,7 +4724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>6</v>
       </c>
@@ -4659,7 +4735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>6</v>
       </c>
@@ -4670,7 +4746,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>8</v>
       </c>
@@ -4681,7 +4757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>8</v>
       </c>
@@ -4692,7 +4768,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>8</v>
       </c>
@@ -4703,7 +4779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>9</v>
       </c>
@@ -4714,7 +4790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>9</v>
       </c>
@@ -4725,7 +4801,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>9</v>
       </c>
@@ -4736,7 +4812,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>3</v>
       </c>
@@ -4747,7 +4823,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>3</v>
       </c>
@@ -4758,7 +4834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>3</v>
       </c>
@@ -4769,7 +4845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>5</v>
       </c>
@@ -4780,7 +4856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>5</v>
       </c>
@@ -4791,7 +4867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>5</v>
       </c>
@@ -4802,7 +4878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>6</v>
       </c>
@@ -4813,7 +4889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>6</v>
       </c>
@@ -4824,7 +4900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>7</v>
       </c>
@@ -4846,7 +4922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>7</v>
       </c>
@@ -4857,7 +4933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>7</v>
       </c>
@@ -4868,7 +4944,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>8</v>
       </c>
@@ -4879,7 +4955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>8</v>
       </c>
@@ -4890,7 +4966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>8</v>
       </c>
@@ -4901,7 +4977,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>9</v>
       </c>
@@ -4912,7 +4988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>9</v>
       </c>
@@ -4923,7 +4999,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>9</v>
       </c>
@@ -4934,7 +5010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>3</v>
       </c>
@@ -4945,7 +5021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>3</v>
       </c>
@@ -4956,7 +5032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>3</v>
       </c>
@@ -4967,7 +5043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>5</v>
       </c>
@@ -4978,7 +5054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>5</v>
       </c>
@@ -4989,7 +5065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>5</v>
       </c>
@@ -5000,7 +5076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>6</v>
       </c>
@@ -5011,7 +5087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>6</v>
       </c>
@@ -5022,7 +5098,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>6</v>
       </c>
@@ -5033,7 +5109,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>7</v>
       </c>
@@ -5044,7 +5120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>7</v>
       </c>
@@ -5055,7 +5131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>7</v>
       </c>
@@ -5066,7 +5142,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>8</v>
       </c>
@@ -5077,7 +5153,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>8</v>
       </c>
@@ -5088,7 +5164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>8</v>
       </c>
@@ -5099,7 +5175,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>9</v>
       </c>
@@ -5110,7 +5186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>9</v>
       </c>
@@ -5121,7 +5197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>9</v>
       </c>
@@ -5137,4 +5213,443 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2245C678-A99A-4C6D-AD32-0F4605BBB432}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>